<commit_message>
Made changes in the path of few files
</commit_message>
<xml_diff>
--- a/Keyword_Driven_Framework_Maven/src/test/java/dataEngine/DataEngine.xlsx
+++ b/Keyword_Driven_Framework_Maven/src/test/java/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17865" windowHeight="4935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17865" windowHeight="2715"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="Page_Name">#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H17"/>
+  <oleSize ref="A1:K8"/>
 </workbook>
 </file>
 
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,7 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H992"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -10830,7 +10830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>